<commit_message>
rev 2.1.1 swap usb micro b to SMT version since many board houses can't make the slots
</commit_message>
<xml_diff>
--- a/debugger2/debugger2.bom.xlsx
+++ b/debugger2/debugger2.bom.xlsx
@@ -336,12 +336,6 @@
     <t>http://www.digikey.com/product-detail/en/CIM21J202NE/1276-6330-1-ND/3973845</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?keywords=609-4618-1-ND</t>
-  </si>
-  <si>
-    <t>USB - micro B USB 2.0 Receptacle Connector 5 Position Surface Mount, Right Angle, Horizontal</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/ABM8-12.000MHZ-B2-T/535-9826-1-ND/2001449</t>
   </si>
   <si>
@@ -421,6 +415,12 @@
   </si>
   <si>
     <t>D4</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/amphenol-fci/10118192-0001LF/609-4613-1-ND/2785378</t>
+  </si>
+  <si>
+    <t>USB - micro B USB 2.0 Receptacle Connector</t>
   </si>
 </sst>
 </file>
@@ -897,17 +897,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1213,10 +1213,10 @@
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1250,10 +1250,10 @@
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1296,10 +1296,10 @@
         <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1322,10 +1322,10 @@
         <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1568,10 +1568,10 @@
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1594,10 +1594,10 @@
         <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1620,10 +1620,10 @@
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1646,10 +1646,10 @@
         <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1672,10 +1672,10 @@
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1698,10 +1698,10 @@
         <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1724,10 +1724,10 @@
         <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1750,24 +1750,24 @@
         <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F46">
         <v>100</v>
       </c>
       <c r="G46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1780,20 +1780,19 @@
     <hyperlink ref="H16" r:id="rId2"/>
     <hyperlink ref="H17" r:id="rId3"/>
     <hyperlink ref="H18" r:id="rId4"/>
-    <hyperlink ref="H21" r:id="rId5"/>
-    <hyperlink ref="H22" r:id="rId6"/>
-    <hyperlink ref="H23" r:id="rId7"/>
-    <hyperlink ref="H25" r:id="rId8"/>
-    <hyperlink ref="H26" r:id="rId9"/>
-    <hyperlink ref="H38" r:id="rId10"/>
-    <hyperlink ref="H39" r:id="rId11"/>
-    <hyperlink ref="H40" r:id="rId12"/>
-    <hyperlink ref="H41" r:id="rId13"/>
-    <hyperlink ref="H42" r:id="rId14"/>
-    <hyperlink ref="H43" r:id="rId15"/>
-    <hyperlink ref="H44" r:id="rId16"/>
-    <hyperlink ref="H45" r:id="rId17"/>
-    <hyperlink ref="H46" r:id="rId18"/>
+    <hyperlink ref="H22" r:id="rId5"/>
+    <hyperlink ref="H23" r:id="rId6"/>
+    <hyperlink ref="H25" r:id="rId7"/>
+    <hyperlink ref="H26" r:id="rId8"/>
+    <hyperlink ref="H38" r:id="rId9"/>
+    <hyperlink ref="H39" r:id="rId10"/>
+    <hyperlink ref="H40" r:id="rId11"/>
+    <hyperlink ref="H41" r:id="rId12"/>
+    <hyperlink ref="H42" r:id="rId13"/>
+    <hyperlink ref="H43" r:id="rId14"/>
+    <hyperlink ref="H44" r:id="rId15"/>
+    <hyperlink ref="H45" r:id="rId16"/>
+    <hyperlink ref="H46" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
change shunt resistor to 0.05 ohm
</commit_message>
<xml_diff>
--- a/debugger2/debugger2.bom.xlsx
+++ b/debugger2/debugger2.bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="217">
   <si>
     <t>Source</t>
   </si>
@@ -629,21 +629,12 @@
     <t>RES SMD 220 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 0.01 OHM 1% 1/2W 1206</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/2176055-1/A109621CT-ND/4032387</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/vishay-dale/CRCW0603220RFKEA/541-220HCT-ND/1179731</t>
   </si>
   <si>
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>RLP73V2BR010FTDF</t>
-  </si>
-  <si>
     <t>CRCW060310R0FKEA</t>
   </si>
   <si>
@@ -675,6 +666,18 @@
   </si>
   <si>
     <t>SWITCH TACTILE SPST-NO 0.02A 15V</t>
+  </si>
+  <si>
+    <t>CSR1206FT50L0</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics</t>
+  </si>
+  <si>
+    <t>RES SMD 0.05 OHM 1% 1/2W 1206</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/stackpole-electronics-inc/CSR1206FT50L0/CSR1206FT50L0CT-ND/3477072</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1047,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1407,10 +1410,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>180</v>
@@ -1734,10 +1737,10 @@
         <v>125</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>44</v>
@@ -1808,10 +1811,10 @@
         <v>125</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>44</v>
@@ -1844,10 +1847,10 @@
         <v>125</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>44</v>
@@ -2015,13 +2018,13 @@
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>61</v>
@@ -2030,7 +2033,7 @@
         <v>139</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="J35" s="3">
         <v>0.01</v>
@@ -2068,7 +2071,7 @@
         <v>139</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J36" s="3">
         <v>220</v>
@@ -2091,13 +2094,13 @@
         <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>105</v>
@@ -2106,7 +2109,7 @@
         <v>139</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>104</v>
@@ -2390,8 +2393,7 @@
     <hyperlink ref="I41" r:id="rId6"/>
     <hyperlink ref="I42" r:id="rId7"/>
     <hyperlink ref="I44" r:id="rId8"/>
-    <hyperlink ref="I35" r:id="rId9"/>
-    <hyperlink ref="I18" r:id="rId10"/>
+    <hyperlink ref="I18" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
swap rpi connector for no paste verison and no stuff
</commit_message>
<xml_diff>
--- a/debugger2/debugger2.bom.xlsx
+++ b/debugger2/debugger2.bom.xlsx
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1566,7 +1566,7 @@
         <v>75</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>165</v>

</xml_diff>

<commit_message>
update U2 and U3 part no on bom and schematic. prevents U2 smoking
</commit_message>
<xml_diff>
--- a/debugger2/debugger2.bom.xlsx
+++ b/debugger2/debugger2.bom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihartwig/repos/raspberrypi-debugger/debugger2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihartwig/repos/rpi-debugger/debugger2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1100" windowWidth="27180" windowHeight="19060" tabRatio="500"/>
+    <workbookView xWindow="13240" yWindow="460" windowWidth="20360" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="debugger2.bom" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="216">
   <si>
     <t>Source</t>
   </si>
@@ -143,9 +143,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>FT2232H</t>
-  </si>
-  <si>
     <t>Housings_QFP:TQFP-64_10x10mm_Pitch0.5mm</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>MIC9409x_SC-70</t>
-  </si>
-  <si>
     <t>TO_SOT_Packages_SMD:SC-70-6</t>
   </si>
   <si>
@@ -575,9 +569,6 @@
     <t>http://www.digikey.com/product-detail/en/93LC56B-I%2FST/93LC56B-I%2FST-ND/319187</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/MIC94093YC6-TR/576-3490-1-ND/2062487</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/FT2232HL-REEL/768-1024-1-ND/1986057</t>
   </si>
   <si>
@@ -599,9 +590,6 @@
     <t>93LC56B-I/ST</t>
   </si>
   <si>
-    <t>MIC94093YC6-TR</t>
-  </si>
-  <si>
     <t>FTDI</t>
   </si>
   <si>
@@ -678,6 +666,15 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/stackpole-electronics-inc/CSR1206FT50L0/CSR1206FT50L0CT-ND/3477072</t>
+  </si>
+  <si>
+    <t>MIC94092YC6-TR</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/microchip-technology/MIC94092YC6-TR/576-3488-1-ND/2062485</t>
+  </si>
+  <si>
+    <t>MIC94092_SC-70</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1145,31 +1142,31 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>20</v>
@@ -1186,29 +1183,29 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="3">
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>30</v>
@@ -1222,25 +1219,25 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" s="3">
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
@@ -1258,29 +1255,29 @@
         <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>30</v>
@@ -1294,29 +1291,29 @@
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>30</v>
@@ -1330,35 +1327,35 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" s="3">
         <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
@@ -1366,37 +1363,37 @@
         <v>6</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" s="3">
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -1404,37 +1401,37 @@
         <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C18" s="3">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
@@ -1442,37 +1439,37 @@
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
@@ -1480,7 +1477,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -1489,20 +1486,20 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
@@ -1516,22 +1513,22 @@
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>25</v>
@@ -1548,37 +1545,37 @@
         <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
@@ -1586,7 +1583,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -1595,20 +1592,20 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
@@ -1616,37 +1613,37 @@
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>169</v>
-      </c>
       <c r="J24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
@@ -1654,37 +1651,37 @@
         <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="F25" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>170</v>
-      </c>
       <c r="J25" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
@@ -1692,35 +1689,35 @@
         <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C26" s="3">
         <v>5</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
@@ -1728,25 +1725,25 @@
         <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="3">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3">
@@ -1756,7 +1753,7 @@
         <v>30</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
@@ -1764,37 +1761,37 @@
         <v>17</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="J28" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
@@ -1802,35 +1799,35 @@
         <v>18</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.15">
@@ -1838,35 +1835,35 @@
         <v>19</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30" s="3">
         <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.15">
@@ -1874,35 +1871,35 @@
         <v>20</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.15">
@@ -1910,35 +1907,35 @@
         <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
@@ -1946,35 +1943,35 @@
         <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" s="3">
         <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.15">
@@ -1982,7 +1979,7 @@
         <v>23</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -1991,20 +1988,20 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.15">
@@ -2012,28 +2009,28 @@
         <v>24</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J35" s="3">
         <v>0.01</v>
@@ -2042,7 +2039,7 @@
         <v>30</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
@@ -2050,28 +2047,28 @@
         <v>25</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J36" s="3">
         <v>220</v>
@@ -2080,7 +2077,7 @@
         <v>30</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
@@ -2088,37 +2085,37 @@
         <v>26</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.15">
@@ -2132,22 +2129,22 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>33</v>
@@ -2164,37 +2161,37 @@
         <v>28</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>55</v>
+        <v>215</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>55</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
@@ -2208,31 +2205,31 @@
         <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="L40" s="3" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.15">
@@ -2240,37 +2237,37 @@
         <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.15">
@@ -2278,37 +2275,37 @@
         <v>31</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
@@ -2316,7 +2313,7 @@
         <v>32</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -2328,17 +2325,17 @@
         <v>34</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
@@ -2346,37 +2343,37 @@
         <v>33</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2388,12 +2385,11 @@
     <hyperlink ref="I24" r:id="rId1"/>
     <hyperlink ref="I25" r:id="rId2"/>
     <hyperlink ref="I38" r:id="rId3"/>
-    <hyperlink ref="I39" r:id="rId4"/>
-    <hyperlink ref="I40" r:id="rId5"/>
-    <hyperlink ref="I41" r:id="rId6"/>
-    <hyperlink ref="I42" r:id="rId7"/>
-    <hyperlink ref="I44" r:id="rId8"/>
-    <hyperlink ref="I18" r:id="rId9"/>
+    <hyperlink ref="I40" r:id="rId4"/>
+    <hyperlink ref="I41" r:id="rId5"/>
+    <hyperlink ref="I42" r:id="rId6"/>
+    <hyperlink ref="I44" r:id="rId7"/>
+    <hyperlink ref="I18" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix D4 D5 part in bom for mismatched footprint, change sch paper size so we plot everything
</commit_message>
<xml_diff>
--- a/debugger2/debugger2.bom.xlsx
+++ b/debugger2/debugger2.bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="217">
   <si>
     <t>Source</t>
   </si>
@@ -563,9 +563,6 @@
     <t>12MHz ±20ppm Crystal 18pF 120 Ohm -20°C ~ 70°C Surface Mount 4-SMD, No Lead (DFN, LCC)</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 200MA</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/93LC56B-I%2FST/93LC56B-I%2FST-ND/319187</t>
   </si>
   <si>
@@ -581,9 +578,6 @@
     <t>http://www.digikey.com/product-detail/en/ABM8-12.000MHZ-B2-T/535-9826-1-ND/2001449</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/CUS520,H3F/CUS520H3FCT-ND/5114381</t>
-  </si>
-  <si>
     <t>Microchip</t>
   </si>
   <si>
@@ -629,12 +623,6 @@
     <t>RES SMD 10 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>Toshiba</t>
-  </si>
-  <si>
-    <t>CUS520,H3F</t>
-  </si>
-  <si>
     <t>CRCW06033K90FKEA</t>
   </si>
   <si>
@@ -675,6 +663,21 @@
   </si>
   <si>
     <t>MIC94092_SC-70</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>DB2S20500L</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 15V 200MA SSMINI2</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/panasonic-electronic-components/DB2S20500L/DB2S20500LCT-ND/2326091</t>
+  </si>
+  <si>
+    <t>Can also use Harwin M20-6102045 (Digikey 952-2219-ND) for bottom TH.</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1358,7 +1361,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>6</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>7</v>
       </c>
@@ -1407,13 +1410,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>105</v>
@@ -1421,8 +1424,8 @@
       <c r="H18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>184</v>
+      <c r="I18" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>104</v>
@@ -1434,7 +1437,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>8</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>9</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>10</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>11</v>
       </c>
@@ -1577,8 +1580,11 @@
       <c r="L22" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M22" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>12</v>
       </c>
@@ -1608,7 +1614,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>13</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>14</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>15</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>16</v>
       </c>
@@ -1734,10 +1740,10 @@
         <v>123</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>43</v>
@@ -1756,7 +1762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>17</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>18</v>
       </c>
@@ -1808,10 +1814,10 @@
         <v>123</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>43</v>
@@ -1830,7 +1836,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>19</v>
       </c>
@@ -1844,10 +1850,10 @@
         <v>123</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>43</v>
@@ -1866,7 +1872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>20</v>
       </c>
@@ -1902,7 +1908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>21</v>
       </c>
@@ -2015,13 +2021,13 @@
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>59</v>
@@ -2030,7 +2036,7 @@
         <v>137</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J35" s="3">
         <v>0.01</v>
@@ -2056,10 +2062,10 @@
         <v>123</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>43</v>
@@ -2068,7 +2074,7 @@
         <v>137</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J36" s="3">
         <v>220</v>
@@ -2091,13 +2097,13 @@
         <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>103</v>
@@ -2106,7 +2112,7 @@
         <v>137</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>102</v>
@@ -2129,10 +2135,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>172</v>
@@ -2144,7 +2150,7 @@
         <v>137</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>33</v>
@@ -2167,10 +2173,10 @@
         <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>173</v>
@@ -2182,16 +2188,16 @@
         <v>137</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
@@ -2205,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>174</v>
@@ -2220,16 +2226,16 @@
         <v>137</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.15">
@@ -2246,7 +2252,7 @@
         <v>169</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>175</v>
@@ -2258,7 +2264,7 @@
         <v>137</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>86</v>
@@ -2281,10 +2287,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>176</v>
@@ -2296,7 +2302,7 @@
         <v>137</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>83</v>
@@ -2349,10 +2355,10 @@
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>177</v>
@@ -2364,7 +2370,7 @@
         <v>137</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>68</v>
@@ -2389,7 +2395,7 @@
     <hyperlink ref="I41" r:id="rId5"/>
     <hyperlink ref="I42" r:id="rId6"/>
     <hyperlink ref="I44" r:id="rId7"/>
-    <hyperlink ref="I18" r:id="rId8"/>
+    <hyperlink ref="I18" r:id="rId8" display="http://www.digikey.com/product-detail/en/CUS520,H3F/CUS520H3FCT-ND/5114381"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>